<commit_message>
[refactor] Modify readme file...
</commit_message>
<xml_diff>
--- a/additional/Reports/report_in_one_sheets_0001.xlsx
+++ b/additional/Reports/report_in_one_sheets_0001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Pycharm\eAssets\additional\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F22085BB-9BF9-4633-9432-DA53BB5EE5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EB4E302-6487-4ADC-B287-4DB134144D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-3465" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17807,7 +17807,7 @@
       <c r="W225" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:V2" xr:uid="{7C6B4C79-CE68-4DCE-BD33-0545B4C87FA3}"/>
+  <autoFilter ref="A2:V2" xr:uid="{3F4A0FC2-D320-42B7-A771-B67F679EB449}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>